<commit_message>
the example for jsp
</commit_message>
<xml_diff>
--- a/jspessentials/src/main/webapp/WEB-INF/books/application_for_leave.xlsx
+++ b/jspessentials/src/main/webapp/WEB-INF/books/application_for_leave.xlsx
@@ -11,26 +11,21 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Applicant">ApplicationForLeave!$C$7</definedName>
+    <definedName name="From">ApplicationForLeave!$D$4</definedName>
+    <definedName name="Reason">ApplicationForLeave!$C$6</definedName>
+    <definedName name="To">ApplicationForLeave!$D$5</definedName>
+    <definedName name="Total">ApplicationForLeave!$F$4</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>APPLICATION FOR LEAVE</t>
-  </si>
-  <si>
-    <t>Applicant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>From</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Period of 
@@ -38,13 +33,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>From</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Days in 
+Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Reason for 
 Leave</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Days in 
-Total</t>
+    <t>Applicant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alex</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -52,7 +63,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Alex</t>
+    <t>Note : This is a simplest demo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -63,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,60 +100,78 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="136"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -237,63 +266,60 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F8"/>
+  <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -608,72 +634,79 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="2:6" ht="29.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:6" ht="25.5">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="4" spans="2:6" ht="24.75" customHeight="1">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>41306</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="18">
-        <v>41306</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="F4" s="16">
         <f>NETWORKDAYS(D4,D5)</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="24" customHeight="1">
-      <c r="B5" s="8"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="2">
         <v>41309</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="14"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:6" ht="54.75" customHeight="1">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" ht="35.25" customHeight="1">
-      <c r="B7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="B7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="2:6" ht="16.5">
-      <c r="C8" s="2"/>
+    <row r="9" spans="2:6" ht="16.5" customHeight="1">
+      <c r="B9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B9:F9"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="E4:E5"/>

</xml_diff>